<commit_message>
Eerste ronde experimentatie af
</commit_message>
<xml_diff>
--- a/experimentatie resultaten/simulated annealing/Tabelresultaten.xlsx
+++ b/experimentatie resultaten/simulated annealing/Tabelresultaten.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tiesv\Documents\RailNLProject\Team-Trein\experimentatie resultaten\simulated annealing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB85509D-DE1E-4C16-AE6C-D2031096B9CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DD68689-CFEB-432F-89E7-52BD9A6410BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6A41B608-95EF-42B6-8E2B-7EC8DAE4784E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>0.4</t>
   </si>
@@ -81,6 +81,24 @@
   </si>
   <si>
     <t>6784.28</t>
+  </si>
+  <si>
+    <t>6787.92</t>
+  </si>
+  <si>
+    <t>6788.92</t>
+  </si>
+  <si>
+    <t>6646.20</t>
+  </si>
+  <si>
+    <t>6806.28</t>
+  </si>
+  <si>
+    <t>6812.20</t>
+  </si>
+  <si>
+    <t>6803.92</t>
   </si>
 </sst>
 </file>
@@ -487,7 +505,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -522,16 +540,25 @@
       <c r="D2" t="s">
         <v>12</v>
       </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
       <c r="C3" t="s">
         <v>9</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -547,6 +574,9 @@
       <c r="D4" t="s">
         <v>14</v>
       </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
@@ -557,6 +587,12 @@
       </c>
       <c r="C5" t="s">
         <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>